<commit_message>
finish notes for 2021-11-08
</commit_message>
<xml_diff>
--- a/academic/Eaton et al. 2021 Plagued by a cryptic clock.xlsx
+++ b/academic/Eaton et al. 2021 Plagued by a cryptic clock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktmea\Projects\obsidian-public\academic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96376A0A-4DBF-4FE1-8759-C00925D841E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCDC712-BBE2-4505-8E18-E7B29D5D6876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table SI 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Table SI 3" sheetId="3" r:id="rId3"/>
     <sheet name="Table SI 4" sheetId="4" r:id="rId4"/>
     <sheet name="Table SI 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Table SI 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="177">
   <si>
     <t xml:space="preserve">   1.ORI    </t>
   </si>
@@ -670,6 +671,62 @@
   </si>
   <si>
     <t>272, 465</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table SI 6. Geographic structure of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Yersinia pestis</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> populations.</t>
+    </r>
+  </si>
+  <si>
+    <t>Continent</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Non-Human Samples</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>Same*</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>* Number of samples with a closest relative collected from the same location.</t>
+  </si>
+  <si>
+    <t>Distinct Locations</t>
+  </si>
+  <si>
+    <t>Total Samples</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1457,6 +1514,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1502,7 +1579,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1697,6 +1774,54 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1730,53 +1855,83 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2136,7 +2291,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2153,17 +2308,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="89.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
@@ -2595,16 +2750,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="72"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="88"/>
     </row>
     <row r="2" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -2973,7 +3128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -2995,15 +3150,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="89" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
       <c r="H1" s="52"/>
       <c r="I1" s="52"/>
       <c r="J1" s="52"/>
@@ -3572,7 +3727,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3591,36 +3746,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="89" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="78"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="94"/>
     </row>
     <row r="2" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="62"/>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="91" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="75" t="s">
+      <c r="C2" s="92"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="91" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="76"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="75" t="s">
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="91" t="s">
         <v>135</v>
       </c>
-      <c r="I2" s="76"/>
-      <c r="J2" s="77"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="93"/>
     </row>
     <row r="3" spans="1:17" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
@@ -4150,7 +4305,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4163,12 +4318,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="89" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
       <c r="E1" s="66"/>
       <c r="F1" s="66"/>
       <c r="G1" s="66"/>
@@ -4178,27 +4333,27 @@
     </row>
     <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="62"/>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="77"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="93"/>
     </row>
     <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="68" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="81" t="s">
+      <c r="E3" s="70" t="s">
         <v>163</v>
       </c>
     </row>
@@ -4206,16 +4361,16 @@
       <c r="A4" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="82">
+      <c r="B4" s="71">
         <v>1867</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="72">
         <v>1875</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="E4" s="88" t="s">
+      <c r="E4" s="77" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4223,16 +4378,16 @@
       <c r="A5" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="84">
+      <c r="B5" s="73">
         <v>1825</v>
       </c>
-      <c r="C5" s="85">
+      <c r="C5" s="74">
         <v>1849</v>
       </c>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="74" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="90" t="s">
+      <c r="E5" s="79" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4240,16 +4395,16 @@
       <c r="A6" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="82">
+      <c r="B6" s="71">
         <v>1759</v>
       </c>
-      <c r="C6" s="83">
+      <c r="C6" s="72">
         <v>1767</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="88" t="s">
+      <c r="E6" s="77" t="s">
         <v>143</v>
       </c>
     </row>
@@ -4257,16 +4412,16 @@
       <c r="A7" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="82">
+      <c r="B7" s="71">
         <v>1279</v>
       </c>
-      <c r="C7" s="83">
+      <c r="C7" s="72">
         <v>1287</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="E7" s="88" t="s">
+      <c r="E7" s="77" t="s">
         <v>145</v>
       </c>
     </row>
@@ -4274,16 +4429,16 @@
       <c r="A8" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="82">
+      <c r="B8" s="71">
         <v>1713</v>
       </c>
-      <c r="C8" s="83">
+      <c r="C8" s="72">
         <v>1750</v>
       </c>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="E8" s="88" t="s">
+      <c r="E8" s="77" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4291,16 +4446,16 @@
       <c r="A9" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="84">
+      <c r="B9" s="73">
         <v>1723</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="74">
         <v>1756</v>
       </c>
-      <c r="D9" s="85" t="s">
+      <c r="D9" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="90" t="s">
+      <c r="E9" s="79" t="s">
         <v>149</v>
       </c>
     </row>
@@ -4308,16 +4463,16 @@
       <c r="A10" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="82">
+      <c r="B10" s="71">
         <v>1927</v>
       </c>
-      <c r="C10" s="83">
+      <c r="C10" s="72">
         <v>1938</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="72" t="s">
         <v>150</v>
       </c>
-      <c r="E10" s="88" t="s">
+      <c r="E10" s="77" t="s">
         <v>151</v>
       </c>
     </row>
@@ -4325,16 +4480,16 @@
       <c r="A11" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="84">
+      <c r="B11" s="73">
         <v>1885</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="74">
         <v>1902</v>
       </c>
-      <c r="D11" s="85" t="s">
+      <c r="D11" s="74" t="s">
         <v>152</v>
       </c>
-      <c r="E11" s="90" t="s">
+      <c r="E11" s="79" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4342,33 +4497,33 @@
       <c r="A12" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="82">
+      <c r="B12" s="71">
         <v>173</v>
       </c>
-      <c r="C12" s="83">
+      <c r="C12" s="72">
         <v>195</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="D12" s="72" t="s">
         <v>154</v>
       </c>
-      <c r="E12" s="88" t="s">
+      <c r="E12" s="77" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="82" t="s">
         <v>164</v>
       </c>
-      <c r="B13" s="82">
+      <c r="B13" s="71">
         <v>386</v>
       </c>
-      <c r="C13" s="83">
+      <c r="C13" s="72">
         <v>399</v>
       </c>
-      <c r="D13" s="83" t="s">
+      <c r="D13" s="72" t="s">
         <v>165</v>
       </c>
-      <c r="E13" s="94">
+      <c r="E13" s="83">
         <v>40474</v>
       </c>
     </row>
@@ -4376,16 +4531,16 @@
       <c r="A14" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="82">
+      <c r="B14" s="71">
         <v>1629</v>
       </c>
-      <c r="C14" s="83">
+      <c r="C14" s="72">
         <v>1658</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="D14" s="72" t="s">
         <v>156</v>
       </c>
-      <c r="E14" s="88" t="s">
+      <c r="E14" s="77" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4393,16 +4548,16 @@
       <c r="A15" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="82">
+      <c r="B15" s="71">
         <v>1767</v>
       </c>
-      <c r="C15" s="83">
+      <c r="C15" s="72">
         <v>1790</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="72" t="s">
         <v>158</v>
       </c>
-      <c r="E15" s="88" t="s">
+      <c r="E15" s="77" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4410,22 +4565,22 @@
       <c r="A16" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="86">
+      <c r="B16" s="75">
         <v>-2852</v>
       </c>
-      <c r="C16" s="87">
+      <c r="C16" s="76">
         <v>-2829</v>
       </c>
-      <c r="D16" s="87" t="s">
+      <c r="D16" s="76" t="s">
         <v>160</v>
       </c>
-      <c r="E16" s="89" t="s">
+      <c r="E16" s="78" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="91"/>
-      <c r="B18" s="92"/>
+      <c r="A18" s="80"/>
+      <c r="B18" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4435,4 +4590,688 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922555F0-DD60-4A30-94C9-BFE9FAE6D9F6}">
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="95" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+    </row>
+    <row r="2" spans="1:15" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="97"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="102" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="102" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="102" t="s">
+        <v>171</v>
+      </c>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="104"/>
+    </row>
+    <row r="3" spans="1:15" s="98" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="110" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="111" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="112" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="108" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="109" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="113" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="116" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="108" t="s">
+        <v>168</v>
+      </c>
+      <c r="I3" s="109" t="s">
+        <v>175</v>
+      </c>
+      <c r="J3" s="113" t="s">
+        <v>172</v>
+      </c>
+      <c r="K3" s="116" t="s">
+        <v>173</v>
+      </c>
+      <c r="L3" s="108" t="s">
+        <v>168</v>
+      </c>
+      <c r="M3" s="109" t="s">
+        <v>175</v>
+      </c>
+      <c r="N3" s="113" t="s">
+        <v>172</v>
+      </c>
+      <c r="O3" s="116" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="106">
+        <v>117</v>
+      </c>
+      <c r="C4" s="107">
+        <v>74</v>
+      </c>
+      <c r="D4" s="105">
+        <v>117</v>
+      </c>
+      <c r="E4" s="106">
+        <v>5</v>
+      </c>
+      <c r="F4" s="114">
+        <v>104</v>
+      </c>
+      <c r="G4" s="107">
+        <v>89</v>
+      </c>
+      <c r="H4" s="105">
+        <v>117</v>
+      </c>
+      <c r="I4" s="106">
+        <v>14</v>
+      </c>
+      <c r="J4" s="114">
+        <v>99</v>
+      </c>
+      <c r="K4" s="107">
+        <v>85</v>
+      </c>
+      <c r="L4" s="105">
+        <v>112</v>
+      </c>
+      <c r="M4" s="106">
+        <v>26</v>
+      </c>
+      <c r="N4" s="114">
+        <v>67</v>
+      </c>
+      <c r="O4" s="107">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="105" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="106">
+        <v>39</v>
+      </c>
+      <c r="C5" s="107">
+        <v>85</v>
+      </c>
+      <c r="D5" s="105">
+        <v>39</v>
+      </c>
+      <c r="E5" s="106">
+        <v>1</v>
+      </c>
+      <c r="F5" s="114">
+        <v>39</v>
+      </c>
+      <c r="G5" s="107">
+        <v>100</v>
+      </c>
+      <c r="H5" s="105">
+        <v>39</v>
+      </c>
+      <c r="I5" s="106">
+        <v>1</v>
+      </c>
+      <c r="J5" s="114">
+        <v>39</v>
+      </c>
+      <c r="K5" s="107">
+        <v>100</v>
+      </c>
+      <c r="L5" s="105">
+        <v>39</v>
+      </c>
+      <c r="M5" s="106">
+        <v>5</v>
+      </c>
+      <c r="N5" s="114">
+        <v>34</v>
+      </c>
+      <c r="O5" s="107">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="105" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="106">
+        <v>4</v>
+      </c>
+      <c r="C6" s="107">
+        <v>50</v>
+      </c>
+      <c r="D6" s="105">
+        <v>4</v>
+      </c>
+      <c r="E6" s="106">
+        <v>1</v>
+      </c>
+      <c r="F6" s="114">
+        <v>4</v>
+      </c>
+      <c r="G6" s="107">
+        <v>100</v>
+      </c>
+      <c r="H6" s="105">
+        <v>4</v>
+      </c>
+      <c r="I6" s="106">
+        <v>3</v>
+      </c>
+      <c r="J6" s="114">
+        <v>2</v>
+      </c>
+      <c r="K6" s="107">
+        <v>50</v>
+      </c>
+      <c r="L6" s="117">
+        <v>1</v>
+      </c>
+      <c r="M6" s="118">
+        <v>1</v>
+      </c>
+      <c r="N6" s="119">
+        <v>0</v>
+      </c>
+      <c r="O6" s="120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="105" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="106">
+        <v>40</v>
+      </c>
+      <c r="C7" s="107">
+        <v>0</v>
+      </c>
+      <c r="D7" s="105">
+        <v>40</v>
+      </c>
+      <c r="E7" s="106">
+        <v>1</v>
+      </c>
+      <c r="F7" s="114">
+        <v>40</v>
+      </c>
+      <c r="G7" s="107">
+        <v>100</v>
+      </c>
+      <c r="H7" s="105">
+        <v>40</v>
+      </c>
+      <c r="I7" s="106">
+        <v>11</v>
+      </c>
+      <c r="J7" s="114">
+        <v>22</v>
+      </c>
+      <c r="K7" s="107">
+        <v>55</v>
+      </c>
+      <c r="L7" s="105">
+        <v>40</v>
+      </c>
+      <c r="M7" s="106">
+        <v>17</v>
+      </c>
+      <c r="N7" s="114">
+        <v>22</v>
+      </c>
+      <c r="O7" s="107">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="105" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="106">
+        <v>116</v>
+      </c>
+      <c r="C8" s="107">
+        <v>85</v>
+      </c>
+      <c r="D8" s="105">
+        <v>116</v>
+      </c>
+      <c r="E8" s="106">
+        <v>2</v>
+      </c>
+      <c r="F8" s="114">
+        <v>88</v>
+      </c>
+      <c r="G8" s="107">
+        <v>76</v>
+      </c>
+      <c r="H8" s="105">
+        <v>116</v>
+      </c>
+      <c r="I8" s="106">
+        <v>9</v>
+      </c>
+      <c r="J8" s="114">
+        <v>70</v>
+      </c>
+      <c r="K8" s="107">
+        <v>60</v>
+      </c>
+      <c r="L8" s="105">
+        <v>110</v>
+      </c>
+      <c r="M8" s="106">
+        <v>38</v>
+      </c>
+      <c r="N8" s="114">
+        <v>37</v>
+      </c>
+      <c r="O8" s="107">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="105" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="106">
+        <v>54</v>
+      </c>
+      <c r="C9" s="107">
+        <v>69</v>
+      </c>
+      <c r="D9" s="105">
+        <v>54</v>
+      </c>
+      <c r="E9" s="106">
+        <v>2</v>
+      </c>
+      <c r="F9" s="114">
+        <v>52</v>
+      </c>
+      <c r="G9" s="107">
+        <v>96</v>
+      </c>
+      <c r="H9" s="105">
+        <v>54</v>
+      </c>
+      <c r="I9" s="106">
+        <v>4</v>
+      </c>
+      <c r="J9" s="114">
+        <v>49</v>
+      </c>
+      <c r="K9" s="107">
+        <v>91</v>
+      </c>
+      <c r="L9" s="105">
+        <v>54</v>
+      </c>
+      <c r="M9" s="106">
+        <v>10</v>
+      </c>
+      <c r="N9" s="114">
+        <v>47</v>
+      </c>
+      <c r="O9" s="107">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="105" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="106">
+        <v>11</v>
+      </c>
+      <c r="C10" s="107">
+        <v>91</v>
+      </c>
+      <c r="D10" s="105">
+        <v>11</v>
+      </c>
+      <c r="E10" s="106">
+        <v>2</v>
+      </c>
+      <c r="F10" s="114">
+        <v>9</v>
+      </c>
+      <c r="G10" s="107">
+        <v>82</v>
+      </c>
+      <c r="H10" s="105">
+        <v>11</v>
+      </c>
+      <c r="I10" s="106">
+        <v>2</v>
+      </c>
+      <c r="J10" s="114">
+        <v>9</v>
+      </c>
+      <c r="K10" s="107">
+        <v>82</v>
+      </c>
+      <c r="L10" s="105">
+        <v>11</v>
+      </c>
+      <c r="M10" s="106">
+        <v>3</v>
+      </c>
+      <c r="N10" s="114">
+        <v>9</v>
+      </c>
+      <c r="O10" s="107">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="105" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="106">
+        <v>11</v>
+      </c>
+      <c r="C11" s="107">
+        <v>91</v>
+      </c>
+      <c r="D11" s="105">
+        <v>11</v>
+      </c>
+      <c r="E11" s="106">
+        <v>1</v>
+      </c>
+      <c r="F11" s="114">
+        <v>11</v>
+      </c>
+      <c r="G11" s="107">
+        <v>100</v>
+      </c>
+      <c r="H11" s="105">
+        <v>11</v>
+      </c>
+      <c r="I11" s="106">
+        <v>2</v>
+      </c>
+      <c r="J11" s="114">
+        <v>11</v>
+      </c>
+      <c r="K11" s="107">
+        <v>100</v>
+      </c>
+      <c r="L11" s="105">
+        <v>11</v>
+      </c>
+      <c r="M11" s="106">
+        <v>7</v>
+      </c>
+      <c r="N11" s="114">
+        <v>5</v>
+      </c>
+      <c r="O11" s="107">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="106">
+        <v>12</v>
+      </c>
+      <c r="C12" s="107">
+        <v>0</v>
+      </c>
+      <c r="D12" s="105">
+        <v>12</v>
+      </c>
+      <c r="E12" s="106">
+        <v>2</v>
+      </c>
+      <c r="F12" s="114">
+        <v>11</v>
+      </c>
+      <c r="G12" s="107">
+        <v>92</v>
+      </c>
+      <c r="H12" s="105">
+        <v>12</v>
+      </c>
+      <c r="I12" s="106">
+        <v>5</v>
+      </c>
+      <c r="J12" s="114">
+        <v>10</v>
+      </c>
+      <c r="K12" s="107">
+        <v>83</v>
+      </c>
+      <c r="L12" s="105">
+        <v>12</v>
+      </c>
+      <c r="M12" s="106">
+        <v>5</v>
+      </c>
+      <c r="N12" s="114">
+        <v>10</v>
+      </c>
+      <c r="O12" s="107">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="105" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="106">
+        <v>103</v>
+      </c>
+      <c r="C13" s="107">
+        <v>100</v>
+      </c>
+      <c r="D13" s="105">
+        <v>103</v>
+      </c>
+      <c r="E13" s="106">
+        <v>1</v>
+      </c>
+      <c r="F13" s="114">
+        <v>103</v>
+      </c>
+      <c r="G13" s="107">
+        <v>100</v>
+      </c>
+      <c r="H13" s="105">
+        <v>103</v>
+      </c>
+      <c r="I13" s="106">
+        <v>2</v>
+      </c>
+      <c r="J13" s="114">
+        <v>100</v>
+      </c>
+      <c r="K13" s="107">
+        <v>97</v>
+      </c>
+      <c r="L13" s="105">
+        <v>99</v>
+      </c>
+      <c r="M13" s="106">
+        <v>4</v>
+      </c>
+      <c r="N13" s="114">
+        <v>95</v>
+      </c>
+      <c r="O13" s="107">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="105" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="106">
+        <v>86</v>
+      </c>
+      <c r="C14" s="107">
+        <v>93</v>
+      </c>
+      <c r="D14" s="105">
+        <v>86</v>
+      </c>
+      <c r="E14" s="106">
+        <v>2</v>
+      </c>
+      <c r="F14" s="114">
+        <v>85</v>
+      </c>
+      <c r="G14" s="107">
+        <v>99</v>
+      </c>
+      <c r="H14" s="105">
+        <v>86</v>
+      </c>
+      <c r="I14" s="106">
+        <v>8</v>
+      </c>
+      <c r="J14" s="114">
+        <v>77</v>
+      </c>
+      <c r="K14" s="107">
+        <v>90</v>
+      </c>
+      <c r="L14" s="105">
+        <v>84</v>
+      </c>
+      <c r="M14" s="106">
+        <v>20</v>
+      </c>
+      <c r="N14" s="114">
+        <v>63</v>
+      </c>
+      <c r="O14" s="107">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="99" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="100">
+        <v>8</v>
+      </c>
+      <c r="C15" s="101">
+        <v>0</v>
+      </c>
+      <c r="D15" s="99">
+        <v>8</v>
+      </c>
+      <c r="E15" s="100">
+        <v>1</v>
+      </c>
+      <c r="F15" s="115">
+        <v>8</v>
+      </c>
+      <c r="G15" s="101">
+        <v>100</v>
+      </c>
+      <c r="H15" s="99">
+        <v>8</v>
+      </c>
+      <c r="I15" s="100">
+        <v>4</v>
+      </c>
+      <c r="J15" s="115">
+        <v>3</v>
+      </c>
+      <c r="K15" s="101">
+        <v>38</v>
+      </c>
+      <c r="L15" s="99">
+        <v>8</v>
+      </c>
+      <c r="M15" s="100">
+        <v>6</v>
+      </c>
+      <c r="N15" s="115">
+        <v>3</v>
+      </c>
+      <c r="O15" s="101">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L2:O2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>